<commit_message>
Création du projet de base avec hierachie de fichiers.
</commit_message>
<xml_diff>
--- a/Conception/Dictionnaire de données.xlsx
+++ b/Conception/Dictionnaire de données.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1532463.SMI\Documents\GitHub\ProjetFinalBD\Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E68FBDB-8A87-4DBB-A15B-CD413DFC5340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95172714-D11F-4728-8FD4-A8C279AEE149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
   <si>
     <t>Champ</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>PRIMARY KEY, FOREIGN KEY</t>
+  </si>
+  <si>
+    <t>couleur</t>
+  </si>
+  <si>
+    <t>CHAR(6)</t>
   </si>
 </sst>
 </file>
@@ -452,6 +458,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -460,15 +475,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,8 +761,8 @@
   </sheetPr>
   <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,18 +773,18 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="G2" s="13" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="G2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -813,7 +819,7 @@
       <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="10"/>
@@ -823,7 +829,7 @@
       <c r="H4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="13" t="s">
         <v>43</v>
       </c>
       <c r="J4" s="10"/>
@@ -835,7 +841,7 @@
       <c r="C5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E5" s="11"/>
@@ -845,7 +851,7 @@
       <c r="H5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="14" t="s">
         <v>42</v>
       </c>
       <c r="J5" s="11"/>
@@ -857,13 +863,13 @@
       <c r="C6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="11"/>
       <c r="G6" s="5"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="17"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -873,49 +879,49 @@
       <c r="C7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="11"/>
       <c r="G7" s="5"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="17"/>
+      <c r="I7" s="14"/>
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="17"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="11"/>
       <c r="G8" s="5"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="17"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="18"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="12"/>
       <c r="G9" s="6"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="18"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="12"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="G11" s="13" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="G11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
@@ -950,7 +956,7 @@
       <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="10"/>
@@ -960,7 +966,7 @@
       <c r="H13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="13" t="s">
         <v>43</v>
       </c>
       <c r="J13" s="10"/>
@@ -972,7 +978,7 @@
       <c r="C14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="11"/>
@@ -982,7 +988,7 @@
       <c r="H14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="14" t="s">
         <v>41</v>
       </c>
       <c r="J14" s="11"/>
@@ -990,7 +996,7 @@
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="17"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="11"/>
       <c r="G15" s="5" t="s">
         <v>27</v>
@@ -998,7 +1004,7 @@
       <c r="H15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="14" t="s">
         <v>42</v>
       </c>
       <c r="J15" s="11"/>
@@ -1006,7 +1012,7 @@
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="17"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="11"/>
       <c r="G16" s="5" t="s">
         <v>28</v>
@@ -1014,43 +1020,43 @@
       <c r="H16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="17"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="17"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="11"/>
       <c r="G17" s="5"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="17"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="18"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="12"/>
       <c r="G18" s="6"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="18"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="12"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="G20" s="13" t="s">
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="G20" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
@@ -1085,7 +1091,7 @@
       <c r="C22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="13" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="10"/>
@@ -1095,7 +1101,7 @@
       <c r="H22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="13" t="s">
         <v>44</v>
       </c>
       <c r="J22" s="10"/>
@@ -1107,7 +1113,7 @@
       <c r="C23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E23" s="11"/>
@@ -1117,7 +1123,7 @@
       <c r="H23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="14" t="s">
         <v>44</v>
       </c>
       <c r="J23" s="11"/>
@@ -1125,57 +1131,57 @@
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="17"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="11"/>
       <c r="G24" s="5"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="17"/>
+      <c r="I24" s="14"/>
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="17"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="11"/>
       <c r="G25" s="5"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="17"/>
+      <c r="I25" s="14"/>
       <c r="J25" s="11"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="17"/>
+      <c r="D26" s="14"/>
       <c r="E26" s="11"/>
       <c r="G26" s="5"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="17"/>
+      <c r="I26" s="14"/>
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="18"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="12"/>
       <c r="G27" s="6"/>
       <c r="H27" s="9"/>
-      <c r="I27" s="18"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="12"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15"/>
-      <c r="G29" s="13" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="G29" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="15"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
@@ -1210,7 +1216,7 @@
       <c r="C31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="10"/>
@@ -1220,7 +1226,7 @@
       <c r="H31" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I31" s="16" t="s">
+      <c r="I31" s="13" t="s">
         <v>43</v>
       </c>
       <c r="J31" s="10"/>
@@ -1232,7 +1238,7 @@
       <c r="C32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E32" s="11"/>
@@ -1242,7 +1248,7 @@
       <c r="H32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="I32" s="14" t="s">
         <v>42</v>
       </c>
       <c r="J32" s="11"/>
@@ -1254,61 +1260,65 @@
       <c r="C33" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="17"/>
+      <c r="D33" s="14"/>
       <c r="E33" s="11"/>
       <c r="G33" s="5"/>
       <c r="H33" s="8"/>
-      <c r="I33" s="17"/>
+      <c r="I33" s="14"/>
       <c r="J33" s="11"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="17"/>
+      <c r="B34" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="14"/>
       <c r="E34" s="11"/>
       <c r="G34" s="5"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="17"/>
+      <c r="I34" s="14"/>
       <c r="J34" s="11"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="17"/>
+      <c r="D35" s="14"/>
       <c r="E35" s="11"/>
       <c r="G35" s="5"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="17"/>
+      <c r="I35" s="14"/>
       <c r="J35" s="11"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="17"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="11"/>
       <c r="G36" s="5"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="17"/>
+      <c r="I36" s="14"/>
       <c r="J36" s="11"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6"/>
       <c r="C37" s="9"/>
-      <c r="D37" s="18"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="12"/>
       <c r="G37" s="6"/>
       <c r="H37" s="9"/>
-      <c r="I37" s="18"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="12"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="15"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
     </row>
     <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
@@ -1331,7 +1341,7 @@
       <c r="C41" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E41" s="10"/>
@@ -1343,7 +1353,7 @@
       <c r="C42" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E42" s="11"/>
@@ -1355,7 +1365,7 @@
       <c r="C43" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E43" s="11"/>
@@ -1367,7 +1377,7 @@
       <c r="C44" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E44" s="11"/>
@@ -1379,7 +1389,7 @@
       <c r="C45" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="17"/>
+      <c r="D45" s="14"/>
       <c r="E45" s="11"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -1389,7 +1399,7 @@
       <c r="C46" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E46" s="11"/>
@@ -1401,7 +1411,7 @@
       <c r="C47" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="18"/>
+      <c r="D47" s="15"/>
       <c r="E47" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renommé table label pour categories
Actualisé les champs correspondant dans les autres tables
</commit_message>
<xml_diff>
--- a/Conception/Dictionnaire de données.xlsx
+++ b/Conception/Dictionnaire de données.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1532463.SMI\Documents\GitHub\ProjetFinalBD\Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95172714-D11F-4728-8FD4-A8C279AEE149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E71118-BB24-4690-BB25-E4B8A048BDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,12 +60,6 @@
     <t>tblRappels</t>
   </si>
   <si>
-    <t>tblLabelTaches</t>
-  </si>
-  <si>
-    <t>tblLabels</t>
-  </si>
-  <si>
     <t>idSession</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>message</t>
   </si>
   <si>
-    <t>idLabel</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
@@ -166,6 +157,15 @@
   </si>
   <si>
     <t>CHAR(6)</t>
+  </si>
+  <si>
+    <t>tblCategories</t>
+  </si>
+  <si>
+    <t>idCategorie</t>
+  </si>
+  <si>
+    <t>tblCategorieTaches</t>
   </si>
 </sst>
 </file>
@@ -761,8 +761,8 @@
   </sheetPr>
   <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,57 +814,57 @@
     </row>
     <row r="4" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E4" s="10"/>
       <c r="G4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E5" s="11"/>
       <c r="G5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" s="11"/>
       <c r="G6" s="5"/>
@@ -874,13 +874,13 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" s="11"/>
       <c r="G7" s="5"/>
@@ -951,45 +951,45 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E14" s="11"/>
       <c r="G14" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J14" s="11"/>
     </row>
@@ -999,13 +999,13 @@
       <c r="D15" s="14"/>
       <c r="E15" s="11"/>
       <c r="G15" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J15" s="11"/>
     </row>
@@ -1015,10 +1015,10 @@
       <c r="D16" s="14"/>
       <c r="E16" s="11"/>
       <c r="G16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="11"/>
@@ -1052,7 +1052,7 @@
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
       <c r="G20" s="16" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
@@ -1086,45 +1086,45 @@
     </row>
     <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E22" s="10"/>
       <c r="G22" s="4" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E23" s="11"/>
       <c r="G23" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J23" s="11"/>
     </row>
@@ -1177,7 +1177,7 @@
       <c r="D29" s="17"/>
       <c r="E29" s="18"/>
       <c r="G29" s="16" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
@@ -1211,54 +1211,54 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" s="4" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E32" s="11"/>
       <c r="G32" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="11"/>
@@ -1269,10 +1269,10 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="11"/>
@@ -1336,80 +1336,80 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E41" s="10"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E42" s="11"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E43" s="11"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E44" s="11"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="11"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C46" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="E46" s="11"/>
     </row>
     <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="12"/>

</xml_diff>

<commit_message>
Ajouter attributs et champs dans les models.
</commit_message>
<xml_diff>
--- a/Conception/Dictionnaire de données.xlsx
+++ b/Conception/Dictionnaire de données.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1532463.SMI\Documents\GitHub\ProjetFinalBD\Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E71118-BB24-4690-BB25-E4B8A048BDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EE408D-E72F-40A7-BB59-F6E42317010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="48">
   <si>
     <t>Champ</t>
   </si>
@@ -96,9 +96,6 @@
     <t>dateFin</t>
   </si>
   <si>
-    <t>valeur</t>
-  </si>
-  <si>
     <t>idRappel</t>
   </si>
   <si>
@@ -166,6 +163,12 @@
   </si>
   <si>
     <t>tblCategorieTaches</t>
+  </si>
+  <si>
+    <t>etat</t>
+  </si>
+  <si>
+    <t>nom</t>
   </si>
 </sst>
 </file>
@@ -761,8 +764,8 @@
   </sheetPr>
   <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,20 +820,20 @@
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="10"/>
       <c r="G4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="10"/>
     </row>
@@ -839,20 +842,20 @@
         <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="11"/>
       <c r="G5" s="5" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" s="11"/>
     </row>
@@ -861,10 +864,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="11"/>
       <c r="G6" s="5"/>
@@ -877,10 +880,10 @@
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="11"/>
       <c r="G7" s="5"/>
@@ -954,20 +957,20 @@
         <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J13" s="10"/>
     </row>
@@ -976,20 +979,20 @@
         <v>15</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="11"/>
       <c r="G14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" s="11"/>
     </row>
@@ -999,13 +1002,13 @@
       <c r="D15" s="14"/>
       <c r="E15" s="11"/>
       <c r="G15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J15" s="11"/>
     </row>
@@ -1015,10 +1018,10 @@
       <c r="D16" s="14"/>
       <c r="E16" s="11"/>
       <c r="G16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="11"/>
@@ -1052,7 +1055,7 @@
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
       <c r="G20" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
@@ -1089,20 +1092,20 @@
         <v>12</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" s="10"/>
       <c r="G22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J22" s="10"/>
     </row>
@@ -1111,20 +1114,20 @@
         <v>16</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="11"/>
       <c r="G23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J23" s="11"/>
     </row>
@@ -1177,7 +1180,7 @@
       <c r="D29" s="17"/>
       <c r="E29" s="18"/>
       <c r="G29" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
@@ -1214,20 +1217,20 @@
         <v>16</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J31" s="10"/>
     </row>
@@ -1236,20 +1239,20 @@
         <v>17</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" s="11"/>
       <c r="G32" s="5" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J32" s="11"/>
     </row>
@@ -1258,7 +1261,7 @@
         <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="11"/>
@@ -1269,10 +1272,10 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="11"/>
@@ -1339,10 +1342,10 @@
         <v>19</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41" s="10"/>
     </row>
@@ -1351,10 +1354,10 @@
         <v>16</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E42" s="11"/>
     </row>
@@ -1363,22 +1366,22 @@
         <v>20</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E43" s="11"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E44" s="11"/>
     </row>
@@ -1387,7 +1390,7 @@
         <v>21</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="11"/>
@@ -1397,10 +1400,10 @@
         <v>22</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E46" s="11"/>
     </row>
@@ -1409,7 +1412,7 @@
         <v>18</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="12"/>

</xml_diff>

<commit_message>
Correction dans les schema BD
</commit_message>
<xml_diff>
--- a/Conception/Dictionnaire de données.xlsx
+++ b/Conception/Dictionnaire de données.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1532463.SMI\Documents\GitHub\ProjetFinalBD\Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EE408D-E72F-40A7-BB59-F6E42317010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB49E43-CF93-456A-83F1-B80FFB47EE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="46">
   <si>
     <t>Champ</t>
   </si>
@@ -66,12 +66,6 @@
     <t>noProgramme</t>
   </si>
   <si>
-    <t>annee</t>
-  </si>
-  <si>
-    <t>saison</t>
-  </si>
-  <si>
     <t>nomProgramme</t>
   </si>
   <si>
@@ -111,12 +105,6 @@
     <t>VARCHAR(6)</t>
   </si>
   <si>
-    <t>SMALLINT</t>
-  </si>
-  <si>
-    <t>VARCHAR(7)</t>
-  </si>
-  <si>
     <t>VARCHAR(50)</t>
   </si>
   <si>
@@ -135,9 +123,6 @@
     <t>DATETIME</t>
   </si>
   <si>
-    <t>PRIMARY KEY, AUTO INCREMENT</t>
-  </si>
-  <si>
     <t>FOREIGN KEY</t>
   </si>
   <si>
@@ -169,6 +154,15 @@
   </si>
   <si>
     <t>nom</t>
+  </si>
+  <si>
+    <t>tblSessionsProgramme</t>
+  </si>
+  <si>
+    <t>VARCHAR(12)</t>
+  </si>
+  <si>
+    <t>ex: Hiver 2022</t>
   </si>
 </sst>
 </file>
@@ -216,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -437,11 +431,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,6 +508,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -764,8 +804,8 @@
   </sheetPr>
   <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +823,7 @@
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
       <c r="G2" s="16" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -820,55 +860,45 @@
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="10"/>
+        <v>34</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>37</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="11"/>
       <c r="G5" s="5" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>38</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="11"/>
       <c r="G6" s="5"/>
       <c r="H6" s="8"/>
@@ -876,15 +906,9 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>38</v>
-      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="11"/>
       <c r="G7" s="5"/>
       <c r="H7" s="8"/>
@@ -920,7 +944,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="18"/>
       <c r="G11" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
@@ -957,42 +981,42 @@
         <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E14" s="11"/>
       <c r="G14" s="5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J14" s="11"/>
     </row>
@@ -1001,15 +1025,9 @@
       <c r="C15" s="8"/>
       <c r="D15" s="14"/>
       <c r="E15" s="11"/>
-      <c r="G15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>38</v>
-      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -1017,12 +1035,8 @@
       <c r="C16" s="8"/>
       <c r="D16" s="14"/>
       <c r="E16" s="11"/>
-      <c r="G16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="14"/>
       <c r="J16" s="11"/>
     </row>
@@ -1055,7 +1069,7 @@
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
       <c r="G20" s="16" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
@@ -1092,42 +1106,42 @@
         <v>12</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E22" s="10"/>
       <c r="G22" s="4" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E23" s="11"/>
       <c r="G23" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J23" s="11"/>
     </row>
@@ -1136,9 +1150,15 @@
       <c r="C24" s="8"/>
       <c r="D24" s="14"/>
       <c r="E24" s="11"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="14"/>
+      <c r="G24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1146,8 +1166,12 @@
       <c r="C25" s="8"/>
       <c r="D25" s="14"/>
       <c r="E25" s="11"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="8"/>
+      <c r="G25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="I25" s="14"/>
       <c r="J25" s="11"/>
     </row>
@@ -1180,7 +1204,7 @@
       <c r="D29" s="17"/>
       <c r="E29" s="18"/>
       <c r="G29" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
@@ -1212,56 +1236,56 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I31" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="D32" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E32" s="11"/>
       <c r="G32" s="5" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="11"/>
@@ -1272,10 +1296,10 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="11"/>
@@ -1294,27 +1318,30 @@
       <c r="I35" s="14"/>
       <c r="J35" s="11"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="8"/>
       <c r="D36" s="14"/>
       <c r="E36" s="11"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="11"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="12"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6"/>
       <c r="C37" s="9"/>
       <c r="D37" s="15"/>
       <c r="E37" s="12"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="12"/>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="21"/>
+    </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="16" t="s">
         <v>8</v>
@@ -1322,6 +1349,18 @@
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="18"/>
+      <c r="G39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
@@ -1336,98 +1375,139 @@
       <c r="E40" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="G40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J40" s="10"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E41" s="10"/>
+      <c r="G41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" s="11"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E42" s="11"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="11"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E43" s="11"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="11"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E44" s="11"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="11"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="11"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G45" s="5"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="11"/>
+    </row>
+    <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E46" s="11"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="12"/>
     </row>
     <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="B29:E29"/>
-    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G38:J38"/>
     <mergeCell ref="B39:E39"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="G29:J29"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="G20:J20"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="59" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correction des diagrammes de BD
</commit_message>
<xml_diff>
--- a/Conception/Dictionnaire de données.xlsx
+++ b/Conception/Dictionnaire de données.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1532463.SMI\Documents\GitHub\ProjetFinalBD\Conception\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuronai\Desktop\CÉGEP\CCHIC\Hiver 2022\Exploitation BD\ProjetFinalBD\Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB49E43-CF93-456A-83F1-B80FFB47EE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91ADBEB2-4571-4716-A8E6-F2D311D9D1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
   <si>
     <t>Champ</t>
   </si>
@@ -45,9 +45,6 @@
     <t>tblProgrammes</t>
   </si>
   <si>
-    <t>tblProgrammeCours</t>
-  </si>
-  <si>
     <t>tblCours</t>
   </si>
   <si>
@@ -156,13 +153,19 @@
     <t>nom</t>
   </si>
   <si>
-    <t>tblSessionsProgramme</t>
-  </si>
-  <si>
     <t>VARCHAR(12)</t>
   </si>
   <si>
     <t>ex: Hiver 2022</t>
+  </si>
+  <si>
+    <t>tblProgrammeSessionCours</t>
+  </si>
+  <si>
+    <t>idCours</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY, AUTO INCREMENT</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -500,6 +503,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -802,13 +814,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J47"/>
+  <dimension ref="B1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="19.140625" customWidth="1"/>
     <col min="7" max="10" width="19.140625" customWidth="1"/>
@@ -816,18 +828,18 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="G2" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="G2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -857,25 +869,25 @@
     </row>
     <row r="4" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="10"/>
     </row>
@@ -885,13 +897,13 @@
       <c r="D5" s="14"/>
       <c r="E5" s="11"/>
       <c r="G5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" s="11"/>
     </row>
@@ -900,9 +912,15 @@
       <c r="C6" s="8"/>
       <c r="D6" s="14"/>
       <c r="E6" s="11"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="14"/>
+      <c r="G6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -937,18 +955,18 @@
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="G11" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="G11" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
@@ -978,45 +996,45 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="11"/>
       <c r="G14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="11"/>
     </row>
@@ -1068,12 +1086,12 @@
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
-      <c r="G20" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="18"/>
+      <c r="G20" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
@@ -1101,84 +1119,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D22" s="13"/>
       <c r="E22" s="10"/>
       <c r="G22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E23" s="11"/>
       <c r="G23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="8"/>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="D24" s="14"/>
       <c r="E24" s="11"/>
       <c r="G24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="8"/>
+      <c r="B25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="D25" s="14"/>
       <c r="E25" s="11"/>
       <c r="G25" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="11"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="14"/>
+    <row r="26" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="E26" s="11"/>
       <c r="G26" s="5"/>
       <c r="H26" s="8"/>
@@ -1186,43 +1216,36 @@
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="6"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="12"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="11"/>
       <c r="G27" s="6"/>
       <c r="H27" s="9"/>
       <c r="I27" s="15"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="6"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="12"/>
+    </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="16" t="s">
+      <c r="G29" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="21"/>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="18"/>
-      <c r="G29" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
       <c r="G30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1236,58 +1259,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="13" t="s">
+    <row r="31" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="G31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="14" t="s">
+      <c r="B32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="11"/>
+      <c r="E32" s="10"/>
       <c r="G32" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="E33" s="11"/>
       <c r="G33" s="5"/>
       <c r="H33" s="8"/>
@@ -1296,12 +1323,14 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="E34" s="11"/>
       <c r="G34" s="5"/>
       <c r="H34" s="8"/>
@@ -1309,9 +1338,15 @@
       <c r="J34" s="11"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="14"/>
+      <c r="B35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="E35" s="11"/>
       <c r="G35" s="5"/>
       <c r="H35" s="8"/>
@@ -1319,8 +1354,12 @@
       <c r="J35" s="11"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
-      <c r="C36" s="8"/>
+      <c r="B36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="D36" s="14"/>
       <c r="E36" s="11"/>
       <c r="G36" s="6"/>
@@ -1329,26 +1368,34 @@
       <c r="J36" s="12"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="6"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="12"/>
+      <c r="B37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="11"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="21"/>
+      <c r="B38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="12"/>
+      <c r="G38" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="24"/>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="18"/>
       <c r="G39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1362,150 +1409,68 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>3</v>
-      </c>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G40" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J40" s="10"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="10"/>
       <c r="G41" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J41" s="11"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E42" s="11"/>
       <c r="G42" s="5"/>
       <c r="H42" s="8"/>
       <c r="I42" s="14"/>
       <c r="J42" s="11"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E43" s="11"/>
       <c r="G43" s="5"/>
       <c r="H43" s="8"/>
       <c r="I43" s="14"/>
       <c r="J43" s="11"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="11"/>
       <c r="G44" s="5"/>
       <c r="H44" s="8"/>
       <c r="I44" s="14"/>
       <c r="J44" s="11"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="11"/>
       <c r="G45" s="5"/>
       <c r="H45" s="8"/>
       <c r="I45" s="14"/>
       <c r="J45" s="11"/>
     </row>
     <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="11"/>
       <c r="G46" s="6"/>
       <c r="H46" s="9"/>
       <c r="I46" s="15"/>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="12"/>
-    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B29:E29"/>
+  <mergeCells count="8">
     <mergeCell ref="G38:J38"/>
-    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B30:E30"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="G20:J20"/>
-    <mergeCell ref="B20:E20"/>
     <mergeCell ref="G29:J29"/>
     <mergeCell ref="G2:J2"/>
   </mergeCells>

</xml_diff>